<commit_message>
Updated DevBoard BOM with Digikey Part Numbers
</commit_message>
<xml_diff>
--- a/Sprite/EagleCAD/Sprite/DevBoard_Files/BOM.xlsx
+++ b/Sprite/EagleCAD/Sprite/DevBoard_Files/BOM.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="37540" yWindow="5280" windowWidth="24740" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="BOM" localSheetId="0">Sheet1!$A$1:$D$33</definedName>
+    <definedName name="BOM" localSheetId="0">Sheet1!$A$1:$D$29</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="94">
   <si>
     <t>Part</t>
   </si>
@@ -255,13 +255,79 @@
   </si>
   <si>
     <t>S2`</t>
+  </si>
+  <si>
+    <t>DigiKey Part Number</t>
+  </si>
+  <si>
+    <t>399-1054-1-ND</t>
+  </si>
+  <si>
+    <t>399-3114-1-ND</t>
+  </si>
+  <si>
+    <t>311-1081-1-ND</t>
+  </si>
+  <si>
+    <t>399-5089-1-ND</t>
+  </si>
+  <si>
+    <t>399-1091-1-ND</t>
+  </si>
+  <si>
+    <t>399-1085-1-ND</t>
+  </si>
+  <si>
+    <t>399-1102-1-ND</t>
+  </si>
+  <si>
+    <t>399-3482-1-ND</t>
+  </si>
+  <si>
+    <t>587-1546-1-ND</t>
+  </si>
+  <si>
+    <t>475-2709-1-ND</t>
+  </si>
+  <si>
+    <t>P56.0KHCT-ND</t>
+  </si>
+  <si>
+    <t>P47.0KHCT-ND</t>
+  </si>
+  <si>
+    <t>P4.70KHCT-ND</t>
+  </si>
+  <si>
+    <t>P270GCT-ND</t>
+  </si>
+  <si>
+    <t>P0.0ACT-ND</t>
+  </si>
+  <si>
+    <t>296-27420-1-ND</t>
+  </si>
+  <si>
+    <t>342-1082-1-ND</t>
+  </si>
+  <si>
+    <t>535-9815-1-ND</t>
+  </si>
+  <si>
+    <t>37T8091</t>
+  </si>
+  <si>
+    <t>*Newark (not stocked by Digikey)</t>
+  </si>
+  <si>
+    <t>*Not stocked by digikey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -293,8 +359,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,6 +381,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,7 +405,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -333,6 +416,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -670,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -682,9 +768,10 @@
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -697,8 +784,11 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -711,8 +801,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -725,8 +818,11 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -739,8 +835,11 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -753,8 +852,11 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -767,8 +869,11 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -781,8 +886,11 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -795,8 +903,11 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -809,8 +920,11 @@
       <c r="D9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -823,8 +937,11 @@
       <c r="D10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -837,8 +954,11 @@
       <c r="D11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -851,8 +971,11 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -865,8 +988,11 @@
       <c r="D13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -879,97 +1005,118 @@
       <c r="D14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E14" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>37</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>37</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
         <v>36</v>
@@ -977,176 +1124,211 @@
       <c r="D21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>69</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>69</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>46</v>
+      </c>
+      <c r="F24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>46</v>
+      </c>
+      <c r="F25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>63</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>64</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>54</v>
+      </c>
+      <c r="E28" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" t="s">
         <v>56</v>
       </c>
+      <c r="E29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Added mfg. Part numbers to BOM
</commit_message>
<xml_diff>
--- a/Sprite/EagleCAD/Sprite/DevBoard_Files/BOM.xlsx
+++ b/Sprite/EagleCAD/Sprite/DevBoard_Files/BOM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="37540" yWindow="5280" windowWidth="24740" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="111">
   <si>
     <t>Part</t>
   </si>
@@ -314,20 +314,71 @@
     <t>535-9815-1-ND</t>
   </si>
   <si>
-    <t>37T8091</t>
-  </si>
-  <si>
-    <t>*Newark (not stocked by Digikey)</t>
-  </si>
-  <si>
-    <t>*Not stocked by digikey</t>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>37T8091 (Newark)</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>C0603C270J5GACTU</t>
+  </si>
+  <si>
+    <t>C0603C474K8PACTU</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R9BB222</t>
+  </si>
+  <si>
+    <t>C0603C104K5RACTU</t>
+  </si>
+  <si>
+    <t>C0603C103K5RACTU</t>
+  </si>
+  <si>
+    <t>C0603C224Z4VACTU</t>
+  </si>
+  <si>
+    <t>C0603C475K9PACTU</t>
+  </si>
+  <si>
+    <t>HK160812NJ-T</t>
+  </si>
+  <si>
+    <t>LG L29K-G2J1-24-Z</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF5602V</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF4702V</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF4701V</t>
+  </si>
+  <si>
+    <t>ERJ-3GEYJ271V</t>
+  </si>
+  <si>
+    <t>ERJ-6GEY0R00V</t>
+  </si>
+  <si>
+    <t>CC430F5137IRGZR</t>
+  </si>
+  <si>
+    <t>HMC5883L-TR</t>
+  </si>
+  <si>
+    <t>ABM11-26.000MHZ-B7G-T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -370,8 +421,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF555555"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,12 +442,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,12 +455,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -417,12 +482,24 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -759,7 +836,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -769,9 +846,10 @@
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -787,8 +865,11 @@
       <c r="E1" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -804,8 +885,11 @@
       <c r="E2" s="7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -821,8 +905,11 @@
       <c r="E3" s="8" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -838,8 +925,11 @@
       <c r="E4" s="7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -855,8 +945,11 @@
       <c r="E5" s="8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -872,8 +965,11 @@
       <c r="E6" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -889,8 +985,11 @@
       <c r="E7" s="8" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -906,8 +1005,11 @@
       <c r="E8" s="7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -923,8 +1025,11 @@
       <c r="E9" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -940,8 +1045,11 @@
       <c r="E10" s="8" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -957,8 +1065,11 @@
       <c r="E11" s="7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -974,8 +1085,11 @@
       <c r="E12" s="8" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -991,8 +1105,11 @@
       <c r="E13" s="8" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1008,8 +1125,11 @@
       <c r="E14" s="8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -1025,8 +1145,11 @@
       <c r="E15" s="8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1041,6 +1164,9 @@
       </c>
       <c r="E16" s="8" t="s">
         <v>82</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1059,6 +1185,9 @@
       <c r="E17" s="8" t="s">
         <v>83</v>
       </c>
+      <c r="F17" s="6" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
@@ -1076,6 +1205,9 @@
       <c r="E18" s="8" t="s">
         <v>84</v>
       </c>
+      <c r="F18" s="6" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
@@ -1093,6 +1225,9 @@
       <c r="E19" s="8" t="s">
         <v>85</v>
       </c>
+      <c r="F19" s="6" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
@@ -1110,6 +1245,9 @@
       <c r="E20" s="8" t="s">
         <v>85</v>
       </c>
+      <c r="F20" s="6" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
@@ -1127,6 +1265,9 @@
       <c r="E21" s="8" t="s">
         <v>86</v>
       </c>
+      <c r="F21" s="6" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
@@ -1144,6 +1285,9 @@
       <c r="E22" s="8" t="s">
         <v>87</v>
       </c>
+      <c r="F22" s="6" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
@@ -1161,6 +1305,9 @@
       <c r="E23" s="8" t="s">
         <v>87</v>
       </c>
+      <c r="F23" s="6" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
@@ -1175,8 +1322,11 @@
       <c r="D24" t="s">
         <v>46</v>
       </c>
-      <c r="F24" t="s">
-        <v>93</v>
+      <c r="E24" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1192,8 +1342,11 @@
       <c r="D25" t="s">
         <v>46</v>
       </c>
-      <c r="F25" t="s">
-        <v>93</v>
+      <c r="E25" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1212,6 +1365,9 @@
       <c r="E26" s="6" t="s">
         <v>88</v>
       </c>
+      <c r="F26" s="6" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
@@ -1229,6 +1385,9 @@
       <c r="E27" s="6" t="s">
         <v>89</v>
       </c>
+      <c r="F27" s="6" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
@@ -1244,10 +1403,10 @@
         <v>54</v>
       </c>
       <c r="E28" t="s">
-        <v>91</v>
-      </c>
-      <c r="F28" t="s">
         <v>92</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1266,6 +1425,9 @@
       <c r="E29" t="s">
         <v>90</v>
       </c>
+      <c r="F29" s="6" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="4" t="s">
@@ -1281,6 +1443,7 @@
         <v>65</v>
       </c>
       <c r="E30" s="5"/>
+      <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="4" t="s">
@@ -1296,6 +1459,7 @@
         <v>65</v>
       </c>
       <c r="E31" s="5"/>
+      <c r="F31" s="10"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="4" t="s">
@@ -1311,8 +1475,9 @@
         <v>65</v>
       </c>
       <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="4" t="s">
         <v>29</v>
       </c>
@@ -1326,6 +1491,7 @@
         <v>65</v>
       </c>
       <c r="E33" s="5"/>
+      <c r="F33" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>